<commit_message>
Occhio all'unità di misura del tempo impiegato!
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/[ERROR]-commesse_release_date.xlsx
+++ b/PS-VRP/Dati_output/[ERROR]-commesse_release_date.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -48,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -416,59 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>release_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>tassativita</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>253393</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>45912.58333333334</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>253392</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>45911.58333333334</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiornato output per mostrare anche commesse tassative problematiche
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/[ERROR]-commesse_release_date.xlsx
+++ b/PS-VRP/Dati_output/[ERROR]-commesse_release_date.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -48,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -416,48 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>release_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>tassativita</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>251889</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>46022.58333333334</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Versione finale 11 settembre
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/[ERROR]-commesse_release_date.xlsx
+++ b/PS-VRP/Dati_output/[ERROR]-commesse_release_date.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,21 +448,23 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>252778</v>
+        <v>253295</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45854.58333333334</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>251889</v>
+        <v>253549</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>46022.58333333334</v>
+        <v>45912.58333333334</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -470,12 +472,221 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>252517</v>
+        <v>253244</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>45855.58333333334</v>
+        <v>45912.58333333334</v>
       </c>
       <c r="C4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>253377</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>252274</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>253371</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>253367</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>253392</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>253525</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>45912.58333333334</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>253376</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>253393</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>45912.58333333334</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>253472</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>45912.58333333334</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>253522</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>252529</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>252397</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>253528</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>253455</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>253436</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>253668</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>244743</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>253261</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>45910.58333333334</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>252741</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>45911.58333333334</v>
+      </c>
+      <c r="C23" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>